<commit_message>
add link objects to the project
</commit_message>
<xml_diff>
--- a/data/spreadsheets/BookChapter.xlsx
+++ b/data/spreadsheets/BookChapter.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBA06F6-A088-FB49-9385-3C72F428F1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61DC0A2-297B-154E-AF54-9E52508E5FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="70940" windowHeight="30120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="500" windowWidth="70940" windowHeight="30120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$30</definedName>
+  </definedNames>
   <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="320">
   <si>
     <t>ID</t>
   </si>
@@ -2843,9 +2846,6 @@
     <t>Fantasy, Identity, Time, Anxiety, Servitude, Domesticity, Chaos, Episodic, Dream-like</t>
   </si>
   <si>
-    <t>Fantasy, Surrealism, Imagination, Contradiction, Fluidity of Space, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Domesticity, Animals, Episodic, Dream-like</t>
-  </si>
-  <si>
     <t>Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals</t>
   </si>
   <si>
@@ -2876,18 +2876,9 @@
     <t>Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Justice, Inverted Justice, Animals, Episodic, Dream-like</t>
   </si>
   <si>
-    <t>Identity</t>
-  </si>
-  <si>
     <t>Identity, Authority, Rules, Tyranny, Absurdity</t>
   </si>
   <si>
-    <t>Fantasy, Identity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Episodic, Dream-like</t>
-  </si>
-  <si>
-    <t>Adventure, Identity, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Domesticity, Animals</t>
-  </si>
-  <si>
     <t>Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Violence, Anger, Judgment, Domesticity, Chaos</t>
   </si>
   <si>
@@ -2907,12 +2898,6 @@
   </si>
   <si>
     <t>Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals</t>
-  </si>
-  <si>
-    <t>Physical Growth, Personal Growth, Transformation, Self-discovery, Chaos, Madness, Confusion</t>
-  </si>
-  <si>
-    <t>Fantasy, Surrealism, Imagination, Contradiction, Fluidity of Space, Identity, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Episodic, Dream-like</t>
   </si>
   <si>
     <t>Fantasy, Identity, Episodic, Dream-like</t>
@@ -3309,6 +3294,24 @@
   </si>
   <si>
     <t>Noémi Villars-Amberg, Daniela Subotic</t>
+  </si>
+  <si>
+    <t>Fantasy, Surrealism, Imagination, Contradiction, Fluidity of Space, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Confusion, Domesticity, Animals, Episodic, Dream-like</t>
+  </si>
+  <si>
+    <t>Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Confusion, Domesticity, Chaos, Animals</t>
+  </si>
+  <si>
+    <t>Fantasy, Identity, Time, Anxiety, Servitude, Chaos, Confusion, Justice, Inverted Justice, Episodic, Dream-like</t>
+  </si>
+  <si>
+    <t>Adventure, Identity, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Confusion, Domesticity, Animals</t>
+  </si>
+  <si>
+    <t>Physical Growth, Personal Growth, Transformation, Self-discovery, Chaos, Confusion</t>
+  </si>
+  <si>
+    <t>Fantasy, Surrealism, Imagination, Contradiction, Fluidity of Space, Identity, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Confusion, Episodic, Dream-like</t>
   </si>
 </sst>
 </file>
@@ -3407,7 +3410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3715,10 +3718,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P30"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A26" sqref="A4:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3736,7 +3740,7 @@
     <col min="16" max="16" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3783,12 +3787,12 @@
         <v>14</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -3797,13 +3801,13 @@
         <v>44</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>92</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>153</v>
@@ -3815,15 +3819,15 @@
         <v>187</v>
       </c>
       <c r="O2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -3835,7 +3839,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F3" t="s">
         <v>53</v>
@@ -3853,24 +3857,24 @@
         <v>120</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>159</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>188</v>
+        <v>314</v>
       </c>
       <c r="O3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -3882,7 +3886,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
@@ -3900,24 +3904,24 @@
         <v>121</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>160</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -3929,7 +3933,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F5" t="s">
         <v>55</v>
@@ -3947,24 +3951,24 @@
         <v>122</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>161</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>189</v>
+        <v>315</v>
       </c>
       <c r="O5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -3976,7 +3980,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="G6" t="s">
         <v>60</v>
@@ -3991,24 +3995,24 @@
         <v>123</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>162</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -4035,24 +4039,24 @@
         <v>124</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>163</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -4082,24 +4086,24 @@
         <v>125</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>164</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O8" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -4111,7 +4115,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G9" t="s">
         <v>63</v>
@@ -4126,24 +4130,24 @@
         <v>126</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>165</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O9" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -4155,7 +4159,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G10" t="s">
         <v>64</v>
@@ -4170,24 +4174,24 @@
         <v>127</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>166</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O10" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
@@ -4214,24 +4218,24 @@
         <v>128</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>167</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O11" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -4243,7 +4247,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="G12" t="s">
         <v>65</v>
@@ -4264,18 +4268,18 @@
         <v>168</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O12" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -4287,7 +4291,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="G13" t="s">
         <v>66</v>
@@ -4308,18 +4312,18 @@
         <v>169</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O13" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
@@ -4346,24 +4350,24 @@
         <v>130</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>170</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O14" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
@@ -4372,16 +4376,16 @@
         <v>45</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="H15" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>154</v>
@@ -4389,19 +4393,16 @@
       <c r="M15" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="N15" s="4" t="s">
-        <v>199</v>
-      </c>
       <c r="O15" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
@@ -4410,13 +4411,13 @@
         <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>106</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>155</v>
@@ -4425,18 +4426,18 @@
         <v>172</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="O16" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
@@ -4445,13 +4446,13 @@
         <v>45</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>107</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>156</v>
@@ -4460,18 +4461,18 @@
         <v>173</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>201</v>
+        <v>316</v>
       </c>
       <c r="O17" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
@@ -4483,13 +4484,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G18" t="s">
         <v>68</v>
       </c>
       <c r="H18" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>108</v>
@@ -4504,18 +4505,18 @@
         <v>174</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>202</v>
+        <v>317</v>
       </c>
       <c r="O18" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B19" t="s">
         <v>32</v>
@@ -4527,13 +4528,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G19" t="s">
         <v>69</v>
       </c>
       <c r="H19" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>109</v>
@@ -4548,18 +4549,18 @@
         <v>175</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="O19" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
@@ -4571,13 +4572,13 @@
         <v>3</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G20" t="s">
         <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>110</v>
@@ -4586,24 +4587,24 @@
         <v>133</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>176</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="O20" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -4615,13 +4616,13 @@
         <v>4</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="G21" t="s">
         <v>71</v>
       </c>
       <c r="H21" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>111</v>
@@ -4636,18 +4637,18 @@
         <v>177</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="O21" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B22" t="s">
         <v>35</v>
@@ -4659,13 +4660,13 @@
         <v>5</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="G22" t="s">
         <v>72</v>
       </c>
       <c r="H22" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>112</v>
@@ -4674,24 +4675,24 @@
         <v>135</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>178</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="O22" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="P22" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
@@ -4709,7 +4710,7 @@
         <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>113</v>
@@ -4724,18 +4725,18 @@
         <v>179</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O23" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
@@ -4747,13 +4748,13 @@
         <v>7</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="G24" t="s">
         <v>74</v>
       </c>
       <c r="H24" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>114</v>
@@ -4768,18 +4769,18 @@
         <v>180</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="O24" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B25" t="s">
         <v>38</v>
@@ -4791,13 +4792,13 @@
         <v>8</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="G25" t="s">
         <v>75</v>
       </c>
       <c r="H25" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>115</v>
@@ -4812,18 +4813,18 @@
         <v>181</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="O25" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
@@ -4835,13 +4836,13 @@
         <v>9</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G26" t="s">
         <v>76</v>
       </c>
       <c r="H26" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>116</v>
@@ -4856,18 +4857,18 @@
         <v>182</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="O26" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="380" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="380" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
@@ -4879,13 +4880,13 @@
         <v>10</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G27" t="s">
         <v>77</v>
       </c>
       <c r="H27" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>117</v>
@@ -4900,18 +4901,18 @@
         <v>183</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>210</v>
+        <v>318</v>
       </c>
       <c r="O27" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="380" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="380" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B28" t="s">
         <v>41</v>
@@ -4929,7 +4930,7 @@
         <v>78</v>
       </c>
       <c r="H28" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>118</v>
@@ -4944,12 +4945,12 @@
         <v>184</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B29" t="s">
         <v>42</v>
@@ -4967,7 +4968,7 @@
         <v>79</v>
       </c>
       <c r="H29" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>119</v>
@@ -4982,18 +4983,18 @@
         <v>185</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>211</v>
+        <v>319</v>
       </c>
       <c r="O29" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B30" t="s">
         <v>43</v>
@@ -5002,10 +5003,10 @@
         <v>45</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="L30" s="4" t="s">
         <v>157</v>
@@ -5014,16 +5015,57 @@
         <v>186</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="O30" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:P30" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="13">
+      <filters>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <x14:filter val="Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Animals"/>
+            <x14:filter val="Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Domesticity, Episodic, Dream-like"/>
+            <x14:filter val="Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Episodic, Dream-like"/>
+            <x14:filter val="Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Justice, Inverted Justice, Animals, Episodic, Dream-like"/>
+            <x14:filter val="Fantasy, Identity, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Domesticity, Animals, Episodic, Dream-like"/>
+            <x14:filter val="Fantasy, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals, Episodic, Dream-like"/>
+            <x14:filter val="Fantasy, Surrealism, Imagination, Contradiction, Fluidity of Space, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals, Episodic, Dream-like"/>
+            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
+            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals"/>
+            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Domesticity, Animals"/>
+            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Wisdom, Mystery, Reflection, Justice, Inverted Justice, Animals"/>
+            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
+            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
+            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals"/>
+            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Time, Anxiety, Servitude, Madness, Confusion, Justice, Inverted Justice, Domesticity, Chaos, Animals"/>
+            <x14:filter val="Surrealism, Imagination, Contradiction, Fluidity of Space, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Madness, Confusion, Violence, Anger, Judgment, Domesticity, Chaos, Animals"/>
+          </mc:Choice>
+          <mc:Fallback>
+            <filter val="Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Animals"/>
+            <filter val="Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Domesticity, Episodic, Dream-like"/>
+            <filter val="Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Episodic, Dream-like"/>
+            <filter val="Fantasy, Identity, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Domesticity, Animals, Episodic, Dream-like"/>
+            <filter val="Fantasy, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals, Episodic, Dream-like"/>
+            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
+            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals"/>
+            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Domesticity, Animals"/>
+            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Wisdom, Mystery, Reflection, Justice, Inverted Justice, Animals"/>
+            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
+            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
+            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals"/>
+            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Time, Anxiety, Servitude, Madness, Confusion, Justice, Inverted Justice, Domesticity, Chaos, Animals"/>
+          </mc:Fallback>
+        </mc:AlternateContent>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -5056,5 +5098,6 @@
     <hyperlink ref="I29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
small updates on alternative texts
</commit_message>
<xml_diff>
--- a/data/spreadsheets/BookChapter.xlsx
+++ b/data/spreadsheets/BookChapter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61DC0A2-297B-154E-AF54-9E52508E5FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BABAB1-6CE3-B34E-91D3-F1021F4551E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="500" windowWidth="70940" windowHeight="30120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29320" yWindow="500" windowWidth="46900" windowHeight="30120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3718,10 +3718,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A26" sqref="A4:A26"/>
     </sheetView>
   </sheetViews>
@@ -3790,7 +3789,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>283</v>
       </c>
@@ -3825,7 +3824,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>284</v>
       </c>
@@ -3919,7 +3918,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>286</v>
       </c>
@@ -4365,7 +4364,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>296</v>
       </c>
@@ -4400,7 +4399,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>297</v>
       </c>
@@ -4435,7 +4434,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>298</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>299</v>
       </c>
@@ -4514,7 +4513,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>300</v>
       </c>
@@ -4866,7 +4865,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="380" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="380" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>308</v>
       </c>
@@ -4910,7 +4909,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="380" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="380" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>309</v>
       </c>
@@ -4948,7 +4947,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>310</v>
       </c>
@@ -4992,7 +4991,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>311</v>
       </c>
@@ -5025,46 +5024,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:P30" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="13">
-      <filters>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <x14:filter val="Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Animals"/>
-            <x14:filter val="Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Domesticity, Episodic, Dream-like"/>
-            <x14:filter val="Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Episodic, Dream-like"/>
-            <x14:filter val="Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Justice, Inverted Justice, Animals, Episodic, Dream-like"/>
-            <x14:filter val="Fantasy, Identity, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Domesticity, Animals, Episodic, Dream-like"/>
-            <x14:filter val="Fantasy, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals, Episodic, Dream-like"/>
-            <x14:filter val="Fantasy, Surrealism, Imagination, Contradiction, Fluidity of Space, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals, Episodic, Dream-like"/>
-            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
-            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals"/>
-            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Domesticity, Animals"/>
-            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Wisdom, Mystery, Reflection, Justice, Inverted Justice, Animals"/>
-            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
-            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
-            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals"/>
-            <x14:filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Time, Anxiety, Servitude, Madness, Confusion, Justice, Inverted Justice, Domesticity, Chaos, Animals"/>
-            <x14:filter val="Surrealism, Imagination, Contradiction, Fluidity of Space, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Madness, Confusion, Violence, Anger, Judgment, Domesticity, Chaos, Animals"/>
-          </mc:Choice>
-          <mc:Fallback>
-            <filter val="Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Animals"/>
-            <filter val="Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Domesticity, Episodic, Dream-like"/>
-            <filter val="Fantasy, Adventure, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Episodic, Dream-like"/>
-            <filter val="Fantasy, Identity, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Domesticity, Animals, Episodic, Dream-like"/>
-            <filter val="Fantasy, Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals, Episodic, Dream-like"/>
-            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
-            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals"/>
-            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Violence, Anger, Judgment, Domesticity, Animals"/>
-            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Wisdom, Mystery, Reflection, Justice, Inverted Justice, Animals"/>
-            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Authority, Rules, Tyranny, Absurdity, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
-            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Logic, Paradoxes, Wordplay, Irony, Time, Anxiety, Servitude, Madness, Confusion, Domesticity, Chaos, Animals"/>
-            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Time, Anxiety, Servitude, Chaos, Madness, Confusion, Justice, Inverted Justice, Animals"/>
-            <filter val="Identity, Physical Growth, Personal Growth, Transformation, Self-discovery, Time, Anxiety, Servitude, Madness, Confusion, Justice, Inverted Justice, Domesticity, Chaos, Animals"/>
-          </mc:Fallback>
-        </mc:AlternateContent>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:P30" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P30">
+      <sortCondition ref="A1:A30"/>
+    </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>